<commit_message>
Update to Form D to change initial info note
</commit_message>
<xml_diff>
--- a/Hluvukani_D_obj_cor/Hluvukani_D_obj_cor-media/Hluvukani_D_obj_cor.xlsx
+++ b/Hluvukani_D_obj_cor/Hluvukani_D_obj_cor-media/Hluvukani_D_obj_cor.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11610" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11610" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -547,95 +547,107 @@
     <t>image</t>
   </si>
   <si>
+    <t>party_id</t>
+  </si>
+  <si>
+    <t>party_id_check</t>
+  </si>
+  <si>
+    <t>Qual é o numero do (co-)titular?</t>
+  </si>
+  <si>
+    <t>Por favor, re-digite o número do (co-)titular como confirmação:</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>Todos os detalhes estão corretos e confirmados</t>
+  </si>
+  <si>
+    <t>outcomes</t>
+  </si>
+  <si>
+    <t>select_one outcomes</t>
+  </si>
+  <si>
+    <t>Por favor, selecione o resultado para esta parcela</t>
+  </si>
+  <si>
+    <t>Foi feita uma objecção que necessita uma resolução ainda</t>
+  </si>
+  <si>
+    <t>O titular não confirmou os seus detalhes durante o período de O &amp; C</t>
+  </si>
+  <si>
+    <t>certify</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>disputed</t>
+  </si>
+  <si>
+    <t>unconfirmed</t>
+  </si>
+  <si>
+    <t>Foi feita uma alteração aos detalhes do(s) (co-)titular(es) ou as limites da parcela</t>
+  </si>
+  <si>
+    <t>O número do titular que reentrou não corresponde à sua primeira entrada. Faça a favor de verificar de novo.</t>
+  </si>
+  <si>
+    <t>.=${party_id}</t>
+  </si>
+  <si>
+    <t>${outcome}='change'</t>
+  </si>
+  <si>
+    <t>limites_new_image</t>
+  </si>
+  <si>
+    <t>Resposta invalida - O campo do nome não pode incluir um novo paragrafo. Faça a favor de eliminar qualquer linha adicional.</t>
+  </si>
+  <si>
+    <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâôàèê]{1,75}$")</t>
+  </si>
+  <si>
+    <t>Hluvukani_D_V2</t>
+  </si>
+  <si>
+    <t>Tire uma fotografia da parcela no mapa, mostrando claramente a mudança nas limites</t>
+  </si>
+  <si>
+    <t>concat('OC','_',${parcel_id})</t>
+  </si>
+  <si>
     <t>&lt;br/&gt; &lt;span style="color:#57b055"&gt;${my_form_name}&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;Este formulário é utilizado para gravar os resultados de processo de Objecções e Correções.
 O técnico pode usar o formulário &lt;br/&gt; &lt;span style="color:#57b055"&gt;depois de conclusão da publicação do edital&lt;/span&gt;.
-O formulário é usado para reportar a necessidade de mudar ou a configuração das parcelas ou mudanças na informação relacionada sobre os titulares. 
-&lt;span style="color:#FF0000"&gt;Se os detalhes de mais de um titular dos co-titulares precisam de ser alterados, o formulário deve ser preenchido uma vez para cada titular&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;
+O formulário é usado para reportar:
+- a necessidade de mudar a configuração dos limites de parcelas
+ou
+- mudanças na informação publicada no edital, relacionada aos titulares
+ou
+- para confirmar a informação publicada no edital, relacionada aos titulares
+&lt;span style="color:#FF0000"&gt;Se houver mais de um titular para uma parcela, o formulário deve ser preenchido uma vez para cada titular&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;
 Por favor deslizar para a frente para continuar.</t>
-  </si>
-  <si>
-    <t>party_id</t>
-  </si>
-  <si>
-    <t>party_id_check</t>
-  </si>
-  <si>
-    <t>Qual é o numero do (co-)titular?</t>
-  </si>
-  <si>
-    <t>Por favor, re-digite o número do (co-)titular como confirmação:</t>
-  </si>
-  <si>
-    <t>outcome</t>
-  </si>
-  <si>
-    <t>Todos os detalhes estão corretos e confirmados</t>
-  </si>
-  <si>
-    <t>outcomes</t>
-  </si>
-  <si>
-    <t>select_one outcomes</t>
-  </si>
-  <si>
-    <t>Por favor, selecione o resultado para esta parcela</t>
-  </si>
-  <si>
-    <t>Foi feita uma objecção que necessita uma resolução ainda</t>
-  </si>
-  <si>
-    <t>O titular não confirmou os seus detalhes durante o período de O &amp; C</t>
-  </si>
-  <si>
-    <t>certify</t>
-  </si>
-  <si>
-    <t>change</t>
-  </si>
-  <si>
-    <t>disputed</t>
-  </si>
-  <si>
-    <t>unconfirmed</t>
-  </si>
-  <si>
-    <t>Foi feita uma alteração aos detalhes do(s) (co-)titular(es) ou as limites da parcela</t>
-  </si>
-  <si>
-    <t>O número do titular que reentrou não corresponde à sua primeira entrada. Faça a favor de verificar de novo.</t>
-  </si>
-  <si>
-    <t>.=${party_id}</t>
-  </si>
-  <si>
-    <t>${outcome}='change'</t>
-  </si>
-  <si>
-    <t>limites_new_image</t>
-  </si>
-  <si>
-    <t>Resposta invalida - O campo do nome não pode incluir um novo paragrafo. Faça a favor de eliminar qualquer linha adicional.</t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâôàèê]{1,75}$")</t>
-  </si>
-  <si>
-    <t>Hluvukani_D_V2</t>
-  </si>
-  <si>
-    <t>Tire uma fotografia da parcela no mapa, mostrando claramente a mudança nas limites</t>
-  </si>
-  <si>
-    <t>concat('OC','_',${parcel_id})</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -805,342 +817,342 @@
   </borders>
   <cellStyleXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="240">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1721,11 +1733,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H7" sqref="H7:I7"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,15 +1826,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="14" customFormat="1" ht="240.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>172</v>
+      <c r="C5" s="44" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1855,11 +1867,11 @@
       <c r="G7" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="I7" s="39" t="s">
+      <c r="H7" s="38" t="s">
         <v>193</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>192</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>21</v>
@@ -1909,16 +1921,16 @@
       </c>
     </row>
     <row r="10" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="B10" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>181</v>
-      </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="38" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1926,13 +1938,13 @@
       <c r="A11" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="J11" s="39" t="s">
+      <c r="B11" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="J11" s="38" t="s">
         <v>21</v>
       </c>
       <c r="L11" s="26" t="s">
@@ -1943,19 +1955,19 @@
       <c r="A12" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="39" t="s">
-        <v>190</v>
-      </c>
-      <c r="I12" s="39" t="s">
+      <c r="B12" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="H12" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="I12" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="J12" s="38" t="s">
         <v>21</v>
       </c>
       <c r="L12" s="26" t="s">
@@ -1972,10 +1984,10 @@
       <c r="C13" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="43" t="s">
-        <v>191</v>
-      </c>
-      <c r="J13" s="39" t="s">
+      <c r="G13" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="J13" s="38" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1992,13 +2004,13 @@
       <c r="G14" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="I14" s="39" t="s">
+      <c r="H14" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="I14" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="J14" s="38" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2015,13 +2027,13 @@
       <c r="G15" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="39" t="s">
-        <v>194</v>
-      </c>
-      <c r="I15" s="39" t="s">
+      <c r="H15" s="38" t="s">
         <v>193</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="I15" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="J15" s="38" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2038,7 +2050,7 @@
       <c r="G16" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="38" t="s">
         <v>21</v>
       </c>
       <c r="L16" s="12" t="s">
@@ -2058,7 +2070,7 @@
       <c r="G17" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="J17" s="39" t="s">
+      <c r="J17" s="38" t="s">
         <v>21</v>
       </c>
       <c r="L17" s="12" t="s">
@@ -2084,7 +2096,7 @@
       <c r="I18" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="38" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2101,7 +2113,7 @@
       <c r="G19" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="J19" s="39" t="s">
+      <c r="J19" s="38" t="s">
         <v>21</v>
       </c>
       <c r="M19" s="25" t="s">
@@ -2112,16 +2124,16 @@
       <c r="A20" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="B20" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>196</v>
+      <c r="B20" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>195</v>
       </c>
       <c r="G20" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="J20" s="39" t="s">
+      <c r="J20" s="38" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2542,47 +2554,47 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="B36" s="42" t="s">
+      <c r="A36" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="C36" s="40" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C37" s="40" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="40" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="B37" s="42" t="s">
+      <c r="B38" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="C37" s="41" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="B38" s="42" t="s">
+      <c r="C38" s="40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="41" t="s">
         <v>186</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C39" s="40" t="s">
         <v>182</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="B39" s="42" t="s">
-        <v>187</v>
-      </c>
-      <c r="C39" s="41" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2815,8 +2827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2847,13 +2859,13 @@
         <v>76</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2" s="13">
-        <v>201709231</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>197</v>
+        <v>201709261</v>
+      </c>
+      <c r="D2" s="43" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New version of O&C Form
</commit_message>
<xml_diff>
--- a/Hluvukani_D_obj_cor/Hluvukani_D_obj_cor-media/Hluvukani_D_obj_cor.xlsx
+++ b/Hluvukani_D_obj_cor/Hluvukani_D_obj_cor-media/Hluvukani_D_obj_cor.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11610" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11610" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="217">
   <si>
     <t>type</t>
   </si>
@@ -196,24 +196,12 @@
     <t>Indique toda a informação que precisa ser alterada</t>
   </si>
   <si>
-    <t>Novo apelido da pessoa</t>
-  </si>
-  <si>
-    <t>Novo nome da pessoa</t>
-  </si>
-  <si>
-    <t>Novo género da pessoa:</t>
-  </si>
-  <si>
     <t>select_one genders</t>
   </si>
   <si>
     <t>select_one documents</t>
   </si>
   <si>
-    <t>Novo numero de documento</t>
-  </si>
-  <si>
     <t>regex(., "^[a-zA-Z0-9. _-]{1,25}$")</t>
   </si>
   <si>
@@ -611,9 +599,6 @@
   </si>
   <si>
     <t>regex(., "^[a-zA-Z0-9. _-éáíóãõúçâôàèê]{1,75}$")</t>
-  </si>
-  <si>
-    <t>Hluvukani_D_V2</t>
   </si>
   <si>
     <t>Tire uma fotografia da parcela no mapa, mostrando claramente a mudança nas limites</t>
@@ -633,14 +618,93 @@
 &lt;span style="color:#FF0000"&gt;Se houver mais de um titular para uma parcela, o formulário deve ser preenchido uma vez para cada titular&lt;/span&gt; &lt;br/&gt;  &lt;br/&gt;
 Por favor deslizar para a frente para continuar.</t>
   </si>
+  <si>
+    <t>select_one regions</t>
+  </si>
+  <si>
+    <t>Selecionar a região (Norte, Central ou Sul)</t>
+  </si>
+  <si>
+    <t>select_one blocos</t>
+  </si>
+  <si>
+    <t>bloco_id</t>
+  </si>
+  <si>
+    <t>Selecionar o bloco</t>
+  </si>
+  <si>
+    <t>region_id=${region_id}</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>no-calendar</t>
+  </si>
+  <si>
+    <t>data_new</t>
+  </si>
+  <si>
+    <t>nasc</t>
+  </si>
+  <si>
+    <t>Mudar o data de nascimento</t>
+  </si>
+  <si>
+    <t>selected(${issues}, 'nasc')</t>
+  </si>
+  <si>
+    <t>parcela</t>
+  </si>
+  <si>
+    <t>Mudar o numero da parcela</t>
+  </si>
+  <si>
+    <t>parcel_id_new</t>
+  </si>
+  <si>
+    <t>Mudar apelido da pessoa para:</t>
+  </si>
+  <si>
+    <t>Mudar nome da pessoa para:</t>
+  </si>
+  <si>
+    <t>Mudar género da pessoa para:</t>
+  </si>
+  <si>
+    <t>Mudar data de nascimento da pessoa para:</t>
+  </si>
+  <si>
+    <t>Mudar o tipo de documento de identificação:</t>
+  </si>
+  <si>
+    <t>Mudar o numero de documento para:</t>
+  </si>
+  <si>
+    <t>selected(${issues}, 'parcela')</t>
+  </si>
+  <si>
+    <t>Hluvukani_D_V3</t>
+  </si>
+  <si>
+    <t>Mudar numero da parcela/registo para:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -817,341 +881,355 @@
   </borders>
   <cellStyleXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="240">
@@ -1731,13 +1809,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1912,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1868,213 +1946,210 @@
         <v>41</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I7" s="38" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J7" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:15" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="B8" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="J8" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="J9" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B10" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C10" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="J8" s="26" t="s">
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="J10" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="L10" s="26" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>48</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="25" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="J10" s="38" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>173</v>
-      </c>
       <c r="C12" s="39" t="s">
-        <v>175</v>
-      </c>
-      <c r="H12" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="I12" s="38" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="J12" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="26" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="13" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" s="42" t="s">
-        <v>190</v>
+        <v>27</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>170</v>
       </c>
       <c r="J13" s="38" t="s">
         <v>21</v>
+      </c>
+      <c r="L13" s="26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>69</v>
+      <c r="B14" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>171</v>
       </c>
       <c r="H14" s="38" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="I14" s="38" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="J14" s="38" t="s">
         <v>21</v>
       </c>
+      <c r="L14" s="26" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="I15" s="38" t="s">
-        <v>192</v>
+        <v>54</v>
+      </c>
+      <c r="G15" s="42" t="s">
+        <v>186</v>
       </c>
       <c r="J15" s="38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="J16" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="H16" s="25"/>
+      <c r="J16" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="12" t="s">
-        <v>32</v>
+      <c r="L16" s="26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>52</v>
+      <c r="C17" s="48" t="s">
+        <v>208</v>
       </c>
       <c r="G17" s="25" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>188</v>
       </c>
       <c r="J17" s="38" t="s">
         <v>21</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -2082,19 +2157,19 @@
         <v>27</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="25" t="s">
         <v>60</v>
       </c>
+      <c r="C18" s="48" t="s">
+        <v>209</v>
+      </c>
       <c r="G18" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="H18" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>188</v>
       </c>
       <c r="J18" s="38" t="s">
         <v>21</v>
@@ -2102,46 +2177,129 @@
     </row>
     <row r="19" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="28" t="s">
-        <v>53</v>
+        <v>61</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>210</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="J19" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M19" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>195</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="J20" s="38" t="s">
+      <c r="L19" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="J20" s="47" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="L20" s="47" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="J21" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="25" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>190</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" s="38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B25" s="23" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2153,13 +2311,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A36" sqref="A36:C39"/>
+      <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,7 +2339,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -2194,10 +2352,10 @@
         <v>17</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -2205,10 +2363,10 @@
         <v>17</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -2216,10 +2374,10 @@
         <v>17</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -2227,10 +2385,10 @@
         <v>17</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -2238,10 +2396,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2249,10 +2407,10 @@
         <v>17</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J8" s="30"/>
     </row>
@@ -2261,10 +2419,10 @@
         <v>17</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J9" s="30"/>
     </row>
@@ -2273,10 +2431,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="J10" s="30"/>
     </row>
@@ -2285,10 +2443,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J11" s="30"/>
     </row>
@@ -2297,10 +2455,10 @@
         <v>17</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J12" s="30"/>
     </row>
@@ -2309,10 +2467,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J13" s="30"/>
     </row>
@@ -2321,10 +2479,10 @@
         <v>17</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J14" s="30"/>
     </row>
@@ -2363,249 +2521,249 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="31" t="s">
         <v>103</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="B25" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>114</v>
-      </c>
       <c r="D25" s="31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C36" s="40" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B38" s="41" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="B39" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="40" t="s">
         <v>178</v>
-      </c>
-      <c r="B39" s="41" t="s">
-        <v>186</v>
-      </c>
-      <c r="C39" s="40" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="35" t="s">
-        <v>133</v>
-      </c>
-      <c r="C41" s="36" t="s">
-        <v>134</v>
+      <c r="B41" s="49" t="s">
+        <v>205</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2613,10 +2771,10 @@
         <v>51</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2624,10 +2782,10 @@
         <v>51</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C43" s="36" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2635,10 +2793,10 @@
         <v>51</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C44" s="36" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2646,10 +2804,10 @@
         <v>51</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C45" s="36" t="s">
-        <v>141</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2657,163 +2815,185 @@
         <v>51</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>53</v>
+        <v>136</v>
+      </c>
+      <c r="C46" s="36" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="34"/>
+      <c r="A47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="49" t="s">
+        <v>202</v>
+      </c>
+      <c r="C47" s="45" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="34" t="s">
-        <v>143</v>
+        <v>51</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>145</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B49" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="C49" s="34" t="s">
-        <v>147</v>
-      </c>
+      <c r="A49" s="34"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="34"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="34"/>
-      <c r="B50" s="35"/>
-      <c r="C50" s="34"/>
+      <c r="A50" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="34" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="B52" s="35" t="s">
-        <v>151</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>152</v>
-      </c>
+      <c r="A52" s="34"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="34"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="34" t="s">
         <v>148</v>
-      </c>
-      <c r="B54" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="C54" s="34" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B55" s="35" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C55" s="34" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B56" s="35" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C56" s="34" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B57" s="35" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C57" s="34" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B58" s="35" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B59" s="35" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C59" s="34" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B60" s="35" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B61" s="35" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>170</v>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2827,8 +3007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,16 +3036,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="C2" s="13">
-        <v>201709261</v>
+        <v>201711011</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>